<commit_message>
done. to add split between day check
</commit_message>
<xml_diff>
--- a/input_data/Requirements_Data_edited.xlsx
+++ b/input_data/Requirements_Data_edited.xlsx
@@ -191,7 +191,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +201,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -240,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -269,6 +299,13 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="3" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -494,7 +531,7 @@
   <dimension ref="A1:E998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -8011,10 +8048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H875"/>
+  <dimension ref="A1:V872"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -8023,15 +8060,17 @@
     <col min="2" max="2" width="5.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.77734375" style="14" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="14" customWidth="1"/>
-    <col min="9" max="17" width="14.44140625" style="14" customWidth="1"/>
-    <col min="18" max="16384" width="12.6640625" style="14"/>
+    <col min="5" max="5" width="6.33203125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="12" style="19" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="14" customWidth="1"/>
+    <col min="8" max="19" width="1.88671875" style="14" customWidth="1"/>
+    <col min="20" max="20" width="2.44140625" style="14" customWidth="1"/>
+    <col min="21" max="21" width="2.5546875" style="14" customWidth="1"/>
+    <col min="22" max="22" width="3" style="14" customWidth="1"/>
+    <col min="23" max="16384" width="12.6640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1">
+    <row r="1" spans="1:22" ht="12.75" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
@@ -8055,7 +8094,7 @@
       </c>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1">
+    <row r="2" spans="1:22" ht="12.75" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>27</v>
       </c>
@@ -8075,10 +8114,18 @@
         <v>5</v>
       </c>
       <c r="G2" s="18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="27"/>
+    </row>
+    <row r="3" spans="1:22" ht="12.75" customHeight="1">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
@@ -8095,13 +8142,18 @@
         <v>8</v>
       </c>
       <c r="F3" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="24"/>
+    </row>
+    <row r="4" spans="1:22" ht="12.75" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>27</v>
       </c>
@@ -8123,8 +8175,12 @@
       <c r="G4" s="15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1">
+      <c r="S4" s="27"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+    </row>
+    <row r="5" spans="1:22" ht="12.75" customHeight="1">
       <c r="A5" s="15" t="s">
         <v>28</v>
       </c>
@@ -8147,7 +8203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1">
+    <row r="6" spans="1:22" ht="12.75" customHeight="1">
       <c r="A6" s="15" t="s">
         <v>28</v>
       </c>
@@ -8170,7 +8226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1">
+    <row r="7" spans="1:22" ht="12.75" customHeight="1">
       <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
@@ -8189,7 +8245,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="18"/>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1">
+    <row r="8" spans="1:22" ht="12.75" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>18</v>
       </c>
@@ -8212,7 +8268,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1">
+    <row r="9" spans="1:22" ht="12.75" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>18</v>
       </c>
@@ -8235,7 +8291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1">
+    <row r="10" spans="1:22" ht="12.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>18</v>
       </c>
@@ -8258,70 +8314,75 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1">
+    <row r="11" spans="1:22" ht="12.75" customHeight="1">
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1">
+    <row r="12" spans="1:22" ht="12.75" customHeight="1">
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1">
+    <row r="13" spans="1:22" ht="12.75" customHeight="1">
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1">
+    <row r="14" spans="1:22" ht="12.75" customHeight="1">
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1">
+    <row r="15" spans="1:22" ht="12.75" customHeight="1">
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1">
+    <row r="16" spans="1:22" ht="12.75" customHeight="1">
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="4:4" ht="12.75" customHeight="1">
+    <row r="17" spans="4:17" ht="12.75" customHeight="1">
       <c r="D17" s="13"/>
     </row>
-    <row r="18" spans="4:4" ht="12.75" customHeight="1">
+    <row r="18" spans="4:17" ht="12.75" customHeight="1">
       <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="4:4" ht="12.75" customHeight="1">
+      <c r="M18" s="26"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+    </row>
+    <row r="19" spans="4:17" ht="12.75" customHeight="1">
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="4:4" ht="12.75" customHeight="1">
+    <row r="20" spans="4:17" ht="12.75" customHeight="1">
       <c r="D20" s="13"/>
     </row>
-    <row r="21" spans="4:4" ht="12.75" customHeight="1">
+    <row r="21" spans="4:17" ht="12.75" customHeight="1">
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="4:4" ht="12.75" customHeight="1">
+    <row r="22" spans="4:17" ht="12.75" customHeight="1">
       <c r="D22" s="13"/>
     </row>
-    <row r="23" spans="4:4" ht="12.75" customHeight="1">
+    <row r="23" spans="4:17" ht="12.75" customHeight="1">
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="4:4" ht="12.75" customHeight="1">
+    <row r="24" spans="4:17" ht="12.75" customHeight="1">
       <c r="D24" s="13"/>
     </row>
-    <row r="25" spans="4:4" ht="12.75" customHeight="1">
+    <row r="25" spans="4:17" ht="12.75" customHeight="1">
       <c r="D25" s="13"/>
     </row>
-    <row r="26" spans="4:4" ht="12.75" customHeight="1">
+    <row r="26" spans="4:17" ht="12.75" customHeight="1">
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="4:4" ht="12.75" customHeight="1">
+    <row r="27" spans="4:17" ht="12.75" customHeight="1">
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="4:4" ht="12.75" customHeight="1">
+    <row r="28" spans="4:17" ht="12.75" customHeight="1">
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="4:4" ht="12.75" customHeight="1">
+    <row r="29" spans="4:17" ht="12.75" customHeight="1">
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="4:4" ht="12.75" customHeight="1">
+    <row r="30" spans="4:17" ht="12.75" customHeight="1">
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="4:4" ht="12.75" customHeight="1">
+    <row r="31" spans="4:17" ht="12.75" customHeight="1">
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="4:4" ht="12.75" customHeight="1">
+    <row r="32" spans="4:17" ht="12.75" customHeight="1">
       <c r="D32" s="13"/>
     </row>
     <row r="33" spans="4:4" ht="12.75" customHeight="1">
@@ -9290,9 +9351,6 @@
     <row r="870" ht="12.75" customHeight="1"/>
     <row r="871" ht="12.75" customHeight="1"/>
     <row r="872" ht="12.75" customHeight="1"/>
-    <row r="873" ht="12.75" customHeight="1"/>
-    <row r="874" ht="12.75" customHeight="1"/>
-    <row r="875" ht="12.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9317,86 +9375,86 @@
       <c r="A1" s="8">
         <v>1</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:11" ht="58.95" customHeight="1">
       <c r="A2" s="8">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" spans="1:11" ht="76.05" customHeight="1">
       <c r="A3" s="8">
         <v>3</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:11" ht="39.450000000000003" customHeight="1">
       <c r="A4" s="8">
         <v>4</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
     </row>
     <row r="9" spans="1:11" ht="77.55" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>